<commit_message>
adding updated Work plan
</commit_message>
<xml_diff>
--- a/pitch - gant.xlsx
+++ b/pitch - gant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashke\Documents\Projects\03_reserve_field_with_map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FBAD40-E95B-4DC0-BB56-EF5331761282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49487A8C-E1E6-4157-948F-A24E3F383553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="49">
   <si>
     <t>Category</t>
   </si>
@@ -163,6 +163,15 @@
   </si>
   <si>
     <t>Name, adress, directions, price, opening hours</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>change CSS - phone compatability</t>
+  </si>
+  <si>
+    <t>PWA - Makes a webpage into an app</t>
   </si>
 </sst>
 </file>
@@ -170,7 +179,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="[$-1000000]h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="[$-1000000]h:mm;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -197,7 +206,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -381,54 +390,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -457,17 +418,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -491,24 +441,132 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
       <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -520,88 +578,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -610,239 +608,133 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1199,11 +1091,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1224,442 +1114,482 @@
       <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="I1" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="46">
         <v>6.25E-2</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="F2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="I2" s="39" t="s">
+      <c r="G2" s="2"/>
+      <c r="I2" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="29" t="s">
+      <c r="A3" s="20"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="47">
         <v>6.25E-2</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="I3" s="15" t="s">
+      <c r="G3" s="2"/>
+      <c r="I3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="29" t="s">
+      <c r="A4" s="20"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="47">
         <v>6.25E-2</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="44" t="s">
+      <c r="F4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="I4" s="16" t="s">
+      <c r="G4" s="2"/>
+      <c r="I4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="29" t="s">
+      <c r="A5" s="20"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="47">
         <v>0.25</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="44" t="s">
+      <c r="F5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
+      <c r="G5" s="2"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="23" t="s">
+      <c r="A6" s="20"/>
+      <c r="B6" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="48">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E6" s="41" t="s">
+      <c r="E6" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="44" t="s">
+      <c r="F6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="I6" s="38" t="s">
+      <c r="G6" s="2"/>
+      <c r="I6" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="29" t="s">
+      <c r="A7" s="20"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="41" t="s">
+      <c r="D7" s="48"/>
+      <c r="E7" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="44" t="s">
+      <c r="F7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="I7" s="37" t="s">
+      <c r="G7" s="2"/>
+      <c r="I7" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="29" t="s">
+      <c r="A8" s="20"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="47">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E8" s="41" t="s">
+      <c r="E8" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="44" t="s">
+      <c r="F8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="I8" s="35" t="s">
+      <c r="G8" s="2"/>
+      <c r="I8" s="11" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="23" t="s">
+      <c r="A9" s="20"/>
+      <c r="B9" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="47">
         <v>0.125</v>
       </c>
-      <c r="E9" s="41" t="s">
+      <c r="E9" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="44" t="s">
+      <c r="F9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="I9" s="36" t="s">
+      <c r="G9" s="2"/>
+      <c r="I9" s="12" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="29" t="s">
+      <c r="A10" s="20"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="47">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E10" s="41" t="s">
+      <c r="E10" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="4"/>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="7"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="29" t="s">
+      <c r="A11" s="21"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="47">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E11" s="41" t="s">
+      <c r="E11" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="4"/>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="47">
         <v>0.16666666666666666</v>
       </c>
-      <c r="E12" s="41" t="s">
+      <c r="E12" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="44" t="s">
+      <c r="F12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="4"/>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="29" t="s">
+      <c r="A13" s="20"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="47">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E13" s="41" t="s">
+      <c r="E13" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="44" t="s">
+      <c r="F13" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="4"/>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="25" t="s">
+      <c r="A14" s="20"/>
+      <c r="B14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="47">
         <v>0.125</v>
       </c>
-      <c r="E14" s="41" t="s">
+      <c r="E14" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="4"/>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="23" t="s">
+      <c r="A15" s="20"/>
+      <c r="B15" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="47">
         <v>0.5</v>
       </c>
-      <c r="E15" s="41" t="s">
+      <c r="E15" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="4"/>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="12"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="29" t="s">
+      <c r="A16" s="23"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="47">
         <v>0.83333333333333337</v>
       </c>
-      <c r="E16" s="41" t="s">
+      <c r="E16" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G16" s="4"/>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="48">
         <v>0.125</v>
       </c>
-      <c r="E17" s="41" t="s">
+      <c r="E17" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="25" t="s">
+      <c r="F17" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="4"/>
+      <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="10"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="30" t="s">
+      <c r="A18" s="18"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="41" t="s">
+      <c r="D18" s="48"/>
+      <c r="E18" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="25" t="s">
+      <c r="F18" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="4"/>
+      <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="47">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E19" s="41" t="s">
+      <c r="E19" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="25" t="s">
+      <c r="F19" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="4"/>
+      <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="29" t="s">
+      <c r="A20" s="24"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="48">
         <v>0.25</v>
       </c>
-      <c r="E20" s="41" t="s">
+      <c r="E20" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="25" t="s">
+      <c r="F20" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="4"/>
+      <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="7"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="29" t="s">
+      <c r="A21" s="21"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="41" t="s">
+      <c r="D21" s="48"/>
+      <c r="E21" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="E22" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="25" t="s">
+      <c r="F22" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="28" t="s">
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="E22" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" s="45" t="s">
+      <c r="C23" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="49">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E23" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="G22" s="5"/>
+      <c r="G23" s="36"/>
+    </row>
+    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="34"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="51">
+        <v>0.125</v>
+      </c>
+      <c r="E24" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="16">
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
     <mergeCell ref="A17:A18"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D17:D18"/>
@@ -1675,7 +1605,7 @@
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B17:B18"/>
   </mergeCells>
-  <conditionalFormatting sqref="F2:G22">
+  <conditionalFormatting sqref="F2:G22 F23:F24">
     <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>$I$4</formula>
     </cfRule>
@@ -1692,7 +1622,7 @@
       <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E22">
+  <conditionalFormatting sqref="E2:E24">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>$I$9</formula>
     </cfRule>

</xml_diff>